<commit_message>
New Changes made to check invalid emails during registration
</commit_message>
<xml_diff>
--- a/src/utilities/ExcelRead.xlsx
+++ b/src/utilities/ExcelRead.xlsx
@@ -18,20 +18,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>vishvesh</t>
+    <t>amdv1991@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,13 +58,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -352,17 +370,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Made changes to loop over excel file and Get email data.
</commit_message>
<xml_diff>
--- a/src/utilities/ExcelRead.xlsx
+++ b/src/utilities/ExcelRead.xlsx
@@ -16,9 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>amdv1991@gmail.com</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>test 2</t>
+  </si>
+  <si>
+    <t>test 1</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -380,17 +386,24 @@
     <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="45">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changes made for comparing actual/expected error message for invalid registration.
</commit_message>
<xml_diff>
--- a/src/utilities/ExcelRead.xlsx
+++ b/src/utilities/ExcelRead.xlsx
@@ -21,10 +21,10 @@
     <t>Email</t>
   </si>
   <si>
-    <t>test 2</t>
+    <t>test 1</t>
   </si>
   <si>
-    <t>test 1</t>
+    <t>test 2</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -393,12 +393,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes Made to write into excel file in "Registration Unsuccessful"
</commit_message>
<xml_diff>
--- a/src/utilities/ExcelRead.xlsx
+++ b/src/utilities/ExcelRead.xlsx
@@ -2,49 +2,55 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>test 1</t>
-  </si>
-  <si>
-    <t>test 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>afljaf</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>fdfsdg</t>
+  </si>
+  <si>
+    <t>afaf;l3</t>
+  </si>
+  <si>
+    <t>4ls;g;</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,28 +70,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+  <cellXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -94,10 +89,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -253,7 +248,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -262,13 +257,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -278,7 +273,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -287,7 +282,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -296,7 +291,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -306,12 +301,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -342,7 +337,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -361,7 +356,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -374,36 +369,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F5" sqref="C3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="26.5703125" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -415,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -427,6 +439,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>